<commit_message>
Altered the create_template.py file so that it creates te template in a different format on a windows machine. Yet to test on windows machine
</commit_message>
<xml_diff>
--- a/autoReport/test_template.xlsx
+++ b/autoReport/test_template.xlsx
@@ -58,8 +58,8 @@
     <t>Fluidigm Image:</t>
   </si>
   <si>
-    <t>The following information is for research purpose only. Any decisions made on the information should be made
-by an appropriate responsible clinician who may require further confirmation within a clinical laboratory.</t>
+    <t>The following information is for research purpose only. Any decisions made on the information should be made by an appropriate
+responsible clinician who may require further confirmation within a clinical laboratory.</t>
   </si>
 </sst>
 </file>
@@ -79,13 +79,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="00000000"/>
-      <sz val="8"/>
+      <sz val="10"/>
     </font>
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="00000000"/>
-      <sz val="10"/>
+      <sz val="14"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -97,14 +97,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="00000000"/>
-      <sz val="18"/>
+      <sz val="20"/>
       <u val="single"/>
     </font>
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="00000000"/>
-      <sz val="12"/>
+      <sz val="8"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,16 +125,16 @@
     </border>
     <border>
       <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
@@ -148,37 +148,34 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="left"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,12 +516,12 @@
       <c r="C7" s="4" t="n"/>
       <c r="D7" s="4" t="n"/>
       <c r="E7" s="4" t="n"/>
-      <c r="F7" s="6" t="n"/>
+      <c r="F7" s="3" t="n"/>
       <c r="G7" s="4" t="n"/>
       <c r="H7" s="4" t="n"/>
       <c r="I7" s="4" t="n"/>
       <c r="J7" s="4" t="n"/>
-      <c r="K7" s="7" t="n"/>
+      <c r="K7" s="6" t="n"/>
     </row>
     <row r="8" spans="1:11">
       <c r="B8" s="5" t="s">
@@ -533,12 +530,12 @@
       <c r="C8" s="4" t="n"/>
       <c r="D8" s="4" t="n"/>
       <c r="E8" s="4" t="n"/>
-      <c r="F8" s="6" t="n"/>
+      <c r="F8" s="3" t="n"/>
       <c r="G8" s="4" t="n"/>
       <c r="H8" s="4" t="n"/>
       <c r="I8" s="4" t="n"/>
       <c r="J8" s="4" t="n"/>
-      <c r="K8" s="7" t="n"/>
+      <c r="K8" s="6" t="n"/>
     </row>
     <row r="9" spans="1:11">
       <c r="B9" s="5" t="s">
@@ -547,18 +544,18 @@
       <c r="C9" s="4" t="n"/>
       <c r="D9" s="4" t="n"/>
       <c r="E9" s="4" t="n"/>
-      <c r="F9" s="8" t="n"/>
-      <c r="J9" s="9" t="n"/>
-      <c r="K9" s="7" t="n"/>
+      <c r="F9" s="7" t="n"/>
+      <c r="J9" s="8" t="n"/>
+      <c r="K9" s="6" t="n"/>
     </row>
     <row r="10" spans="1:11">
       <c r="B10" s="5" t="n"/>
       <c r="C10" s="4" t="n"/>
       <c r="D10" s="4" t="n"/>
       <c r="E10" s="4" t="n"/>
-      <c r="F10" s="8" t="n"/>
-      <c r="J10" s="9" t="n"/>
-      <c r="K10" s="7" t="n"/>
+      <c r="F10" s="7" t="n"/>
+      <c r="J10" s="8" t="n"/>
+      <c r="K10" s="6" t="n"/>
     </row>
     <row r="11" spans="1:11">
       <c r="B11" s="5" t="s">
@@ -567,12 +564,12 @@
       <c r="C11" s="4" t="n"/>
       <c r="D11" s="4" t="n"/>
       <c r="E11" s="4" t="n"/>
-      <c r="F11" s="6" t="n"/>
+      <c r="F11" s="3" t="n"/>
       <c r="G11" s="4" t="n"/>
       <c r="H11" s="4" t="n"/>
       <c r="I11" s="4" t="n"/>
       <c r="J11" s="4" t="n"/>
-      <c r="K11" s="7" t="n"/>
+      <c r="K11" s="6" t="n"/>
     </row>
     <row r="12" spans="1:11">
       <c r="B12" s="5" t="s">
@@ -581,12 +578,12 @@
       <c r="C12" s="4" t="n"/>
       <c r="D12" s="4" t="n"/>
       <c r="E12" s="4" t="n"/>
-      <c r="F12" s="6" t="n"/>
+      <c r="F12" s="3" t="n"/>
       <c r="G12" s="4" t="n"/>
       <c r="H12" s="4" t="n"/>
       <c r="I12" s="4" t="n"/>
       <c r="J12" s="4" t="n"/>
-      <c r="K12" s="7" t="n"/>
+      <c r="K12" s="6" t="n"/>
     </row>
     <row r="13" spans="1:11">
       <c r="B13" s="5" t="s">
@@ -595,12 +592,12 @@
       <c r="C13" s="4" t="n"/>
       <c r="D13" s="4" t="n"/>
       <c r="E13" s="4" t="n"/>
-      <c r="F13" s="6" t="n"/>
+      <c r="F13" s="3" t="n"/>
       <c r="G13" s="4" t="n"/>
       <c r="H13" s="4" t="n"/>
       <c r="I13" s="4" t="n"/>
       <c r="J13" s="4" t="n"/>
-      <c r="K13" s="7" t="n"/>
+      <c r="K13" s="6" t="n"/>
     </row>
     <row r="14" spans="1:11">
       <c r="B14" s="5" t="s">
@@ -609,12 +606,12 @@
       <c r="C14" s="4" t="n"/>
       <c r="D14" s="4" t="n"/>
       <c r="E14" s="4" t="n"/>
-      <c r="F14" s="6" t="n"/>
+      <c r="F14" s="3" t="n"/>
       <c r="G14" s="4" t="n"/>
       <c r="H14" s="4" t="n"/>
       <c r="I14" s="4" t="n"/>
       <c r="J14" s="4" t="n"/>
-      <c r="K14" s="7" t="n"/>
+      <c r="K14" s="6" t="n"/>
     </row>
     <row r="15" spans="1:11">
       <c r="B15" s="5" t="s">
@@ -623,12 +620,12 @@
       <c r="C15" s="4" t="n"/>
       <c r="D15" s="4" t="n"/>
       <c r="E15" s="4" t="n"/>
-      <c r="F15" s="6" t="n"/>
+      <c r="F15" s="3" t="n"/>
       <c r="G15" s="4" t="n"/>
       <c r="H15" s="4" t="n"/>
       <c r="I15" s="4" t="n"/>
       <c r="J15" s="4" t="n"/>
-      <c r="K15" s="7" t="n"/>
+      <c r="K15" s="6" t="n"/>
     </row>
     <row r="16" spans="1:11">
       <c r="B16" s="5" t="s">
@@ -637,15 +634,15 @@
       <c r="C16" s="4" t="n"/>
       <c r="D16" s="4" t="n"/>
       <c r="E16" s="4" t="n"/>
-      <c r="F16" s="10" t="n"/>
+      <c r="F16" s="9" t="n"/>
       <c r="G16" s="4" t="n"/>
       <c r="H16" s="4" t="n"/>
       <c r="I16" s="4" t="n"/>
       <c r="J16" s="4" t="n"/>
-      <c r="K16" s="7" t="n"/>
+      <c r="K16" s="6" t="n"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="B17" s="11" t="n"/>
+      <c r="B17" s="10" t="n"/>
       <c r="C17" s="4" t="n"/>
       <c r="D17" s="4" t="n"/>
       <c r="E17" s="4" t="n"/>
@@ -654,10 +651,10 @@
       <c r="H17" s="4" t="n"/>
       <c r="I17" s="4" t="n"/>
       <c r="J17" s="4" t="n"/>
-      <c r="K17" s="7" t="n"/>
+      <c r="K17" s="6" t="n"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="B18" s="11" t="n"/>
+      <c r="B18" s="10" t="n"/>
       <c r="C18" s="4" t="n"/>
       <c r="D18" s="4" t="n"/>
       <c r="E18" s="4" t="n"/>
@@ -666,10 +663,10 @@
       <c r="H18" s="4" t="n"/>
       <c r="I18" s="4" t="n"/>
       <c r="J18" s="4" t="n"/>
-      <c r="K18" s="7" t="n"/>
+      <c r="K18" s="6" t="n"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="B19" s="11" t="n"/>
+      <c r="B19" s="10" t="n"/>
       <c r="C19" s="4" t="n"/>
       <c r="D19" s="4" t="n"/>
       <c r="E19" s="4" t="n"/>
@@ -678,10 +675,10 @@
       <c r="H19" s="4" t="n"/>
       <c r="I19" s="4" t="n"/>
       <c r="J19" s="4" t="n"/>
-      <c r="K19" s="7" t="n"/>
+      <c r="K19" s="6" t="n"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="B20" s="11" t="n"/>
+      <c r="B20" s="10" t="n"/>
       <c r="C20" s="4" t="n"/>
       <c r="D20" s="4" t="n"/>
       <c r="E20" s="4" t="n"/>
@@ -690,7 +687,7 @@
       <c r="H20" s="4" t="n"/>
       <c r="I20" s="4" t="n"/>
       <c r="J20" s="4" t="n"/>
-      <c r="K20" s="7" t="n"/>
+      <c r="K20" s="6" t="n"/>
     </row>
     <row customHeight="1" ht="18" r="21" spans="1:11">
       <c r="B21" s="2" t="s">
@@ -703,7 +700,7 @@
       </c>
     </row>
     <row r="47" spans="1:11">
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="11" t="s">
         <v>14</v>
       </c>
     </row>
@@ -711,11 +708,11 @@
   <mergeCells count="27">
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="F4:J4"/>
+    <mergeCell ref="F16:J20"/>
+    <mergeCell ref="B47:J48"/>
     <mergeCell ref="B16:E20"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F16:J20"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B47:J48"/>
+    <mergeCell ref="B33:E33"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>

</xml_diff>